<commit_message>
End of day 1
What we have done at the end of day 1, Some branches will still have to be merged but it will be done tomorrow.
</commit_message>
<xml_diff>
--- a/Sprint 2/Sprint_Backlog/Sprint 2 Backlog .xlsx
+++ b/Sprint 2/Sprint_Backlog/Sprint 2 Backlog .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stormfront/Desktop/GITHUB/Sites/DCDLEAFY.github.io/Sprint 2/Sprint_Backlog/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B5BAD599-D85F-D34B-9491-49E0D9D7758B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B586170-A4DB-D340-A515-983246BFD8F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25380" windowHeight="14440" xr2:uid="{534C34EA-1E67-7A49-A34F-DDDABC004054}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="47">
   <si>
     <t>Status</t>
   </si>
@@ -240,13 +240,171 @@
   </si>
   <si>
     <t>Incompleted || 02/02</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>3=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>2=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>2=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="2" tint="-0.499984740745262"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>2=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="2" tint="-0.499984740745262"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>1</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="14">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -309,6 +467,30 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="2" tint="-0.499984740745262"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="5" tint="-0.249977111117893"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri (Body)"/>
     </font>
   </fonts>
   <fills count="12">
@@ -542,27 +724,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -573,6 +734,48 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -580,27 +783,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -917,13 +1099,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B87E7FF6-10D9-A640-9FCB-92C9939F9B69}">
-  <dimension ref="A2:N30"/>
+  <dimension ref="A2:N29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="110" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="82.83203125" customWidth="1"/>
     <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
@@ -940,29 +1122,29 @@
     <col min="14" max="14" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13">
       <c r="B2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
       <c r="F2" s="25"/>
-      <c r="G2" s="32" t="s">
+      <c r="G2" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
-      <c r="M2" s="30" t="s">
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="45" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13">
       <c r="B3" s="8" t="s">
         <v>7</v>
       </c>
@@ -975,7 +1157,7 @@
       <c r="E3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="33" t="s">
+      <c r="F3" s="26" t="s">
         <v>1</v>
       </c>
       <c r="G3" s="2" t="s">
@@ -996,13 +1178,13 @@
       <c r="L3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="M3" s="31"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="41" t="s">
+      <c r="M3" s="46"/>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="29" t="s">
         <v>26</v>
       </c>
       <c r="C4" s="10">
@@ -1014,8 +1196,10 @@
       <c r="E4" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="F4" s="34"/>
-      <c r="G4" s="10"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="10" t="s">
+        <v>43</v>
+      </c>
       <c r="H4" s="10"/>
       <c r="I4" s="10"/>
       <c r="J4" s="10"/>
@@ -1023,9 +1207,9 @@
       <c r="L4" s="10"/>
       <c r="M4" s="16"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="42"/>
-      <c r="B5" s="37" t="s">
+    <row r="5" spans="1:13">
+      <c r="A5" s="49"/>
+      <c r="B5" s="30" t="s">
         <v>27</v>
       </c>
       <c r="C5" s="4">
@@ -1035,10 +1219,12 @@
         <v>4</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="F5" s="35"/>
-      <c r="G5" s="4"/>
+        <v>42</v>
+      </c>
+      <c r="F5" s="28"/>
+      <c r="G5" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
@@ -1046,9 +1232,9 @@
       <c r="L5" s="4"/>
       <c r="M5" s="15"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="42"/>
-      <c r="B6" s="38" t="s">
+    <row r="6" spans="1:13">
+      <c r="A6" s="49"/>
+      <c r="B6" s="31" t="s">
         <v>28</v>
       </c>
       <c r="C6" s="3">
@@ -1060,7 +1246,7 @@
       <c r="E6" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="35"/>
+      <c r="F6" s="28"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
@@ -1069,9 +1255,9 @@
       <c r="L6" s="3"/>
       <c r="M6" s="16"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="42"/>
-      <c r="B7" s="37" t="s">
+    <row r="7" spans="1:13">
+      <c r="A7" s="49"/>
+      <c r="B7" s="30" t="s">
         <v>29</v>
       </c>
       <c r="C7" s="4">
@@ -1083,7 +1269,7 @@
       <c r="E7" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="F7" s="35"/>
+      <c r="F7" s="28"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
@@ -1092,9 +1278,9 @@
       <c r="L7" s="4"/>
       <c r="M7" s="15"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="42"/>
-      <c r="B8" s="38" t="s">
+    <row r="8" spans="1:13">
+      <c r="A8" s="49"/>
+      <c r="B8" s="31" t="s">
         <v>30</v>
       </c>
       <c r="C8" s="3">
@@ -1106,7 +1292,7 @@
       <c r="E8" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="35"/>
+      <c r="F8" s="28"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
@@ -1115,9 +1301,9 @@
       <c r="L8" s="3"/>
       <c r="M8" s="16"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="42"/>
-      <c r="B9" s="37" t="s">
+    <row r="9" spans="1:13">
+      <c r="A9" s="49"/>
+      <c r="B9" s="30" t="s">
         <v>31</v>
       </c>
       <c r="C9" s="4">
@@ -1129,8 +1315,10 @@
       <c r="E9" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="F9" s="35"/>
-      <c r="G9" s="4"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
@@ -1138,9 +1326,9 @@
       <c r="L9" s="4"/>
       <c r="M9" s="15"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="42"/>
-      <c r="B10" s="38" t="s">
+    <row r="10" spans="1:13">
+      <c r="A10" s="49"/>
+      <c r="B10" s="31" t="s">
         <v>32</v>
       </c>
       <c r="C10" s="3">
@@ -1152,7 +1340,7 @@
       <c r="E10" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="F10" s="35"/>
+      <c r="F10" s="28"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
@@ -1161,9 +1349,9 @@
       <c r="L10" s="3"/>
       <c r="M10" s="16"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="42"/>
-      <c r="B11" s="37" t="s">
+    <row r="11" spans="1:13">
+      <c r="A11" s="49"/>
+      <c r="B11" s="30" t="s">
         <v>33</v>
       </c>
       <c r="C11" s="4">
@@ -1173,9 +1361,9 @@
         <v>4</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="F11" s="35"/>
+        <v>36</v>
+      </c>
+      <c r="F11" s="28"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
@@ -1184,9 +1372,9 @@
       <c r="L11" s="4"/>
       <c r="M11" s="15"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="42"/>
-      <c r="B12" s="38" t="s">
+    <row r="12" spans="1:13">
+      <c r="A12" s="49"/>
+      <c r="B12" s="31" t="s">
         <v>34</v>
       </c>
       <c r="C12" s="3">
@@ -1198,8 +1386,10 @@
       <c r="E12" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="F12" s="35"/>
-      <c r="G12" s="3"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
@@ -1207,9 +1397,9 @@
       <c r="L12" s="3"/>
       <c r="M12" s="16"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A13" s="43"/>
-      <c r="B13" s="39" t="s">
+    <row r="13" spans="1:13">
+      <c r="A13" s="50"/>
+      <c r="B13" s="32" t="s">
         <v>35</v>
       </c>
       <c r="C13" s="4">
@@ -1221,7 +1411,7 @@
       <c r="E13" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="F13" s="35"/>
+      <c r="F13" s="28"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
@@ -1230,11 +1420,11 @@
       <c r="L13" s="5"/>
       <c r="M13" s="17"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="40"/>
+    <row r="14" spans="1:13">
+      <c r="A14" s="33"/>
       <c r="C14" s="21"/>
       <c r="D14" s="21"/>
-      <c r="E14" s="28" t="s">
+      <c r="E14" s="43" t="s">
         <v>17</v>
       </c>
       <c r="F14" s="23" t="s">
@@ -1254,36 +1444,38 @@
       </c>
       <c r="K14" s="21"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" s="40"/>
+    <row r="15" spans="1:13">
+      <c r="A15" s="33"/>
       <c r="C15" s="20"/>
       <c r="D15" s="20"/>
-      <c r="E15" s="29"/>
+      <c r="E15" s="44"/>
       <c r="F15" s="24">
         <f>SUM(D4:D13)</f>
         <v>40</v>
       </c>
       <c r="G15" s="22">
-        <f>F15-SUM(G4:G13)</f>
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="H15" s="22">
         <f>G15-SUM(H4:H13)</f>
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="I15" s="22">
         <f>H15-SUM(I4:I13)</f>
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="J15" s="24">
         <f>I15-SUM(J4:J13)</f>
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="K15" s="20"/>
+      <c r="L15" s="12" t="s">
+        <v>41</v>
+      </c>
       <c r="M15" s="18"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A16" s="40"/>
+    <row r="16" spans="1:13" ht="21">
+      <c r="A16" s="33"/>
       <c r="C16" s="19"/>
       <c r="D16" s="19"/>
       <c r="E16" s="19"/>
@@ -1293,12 +1485,23 @@
       <c r="I16" s="20"/>
       <c r="J16" s="20"/>
       <c r="K16" s="19"/>
+      <c r="L16" s="35" t="s">
+        <v>40</v>
+      </c>
       <c r="M16" s="18"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A17" s="40"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" ht="21">
+      <c r="A17" s="33"/>
+      <c r="L17" s="36" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="21">
+      <c r="L18" s="37" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="21">
       <c r="B19" s="14" t="s">
         <v>25</v>
       </c>
@@ -1307,34 +1510,40 @@
       </c>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="L19" s="38" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="21">
       <c r="B20" s="13"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="26"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C20" s="41"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="41"/>
+      <c r="L20" s="39" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="21">
       <c r="B21" s="13"/>
-      <c r="C21" s="26"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="26"/>
+      <c r="C21" s="41"/>
+      <c r="D21" s="41"/>
+      <c r="E21" s="41"/>
+      <c r="L21" s="40" t="s">
+        <v>39</v>
+      </c>
       <c r="N21" s="18"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14">
       <c r="B22" s="13"/>
-      <c r="C22" s="26"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="26"/>
+      <c r="C22" s="41"/>
+      <c r="D22" s="41"/>
+      <c r="E22" s="41"/>
       <c r="N22" s="18"/>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14">
       <c r="N23" s="18"/>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B24" s="12" t="s">
-        <v>41</v>
-      </c>
+    <row r="24" spans="1:14">
       <c r="C24" s="18"/>
       <c r="D24" s="18"/>
       <c r="E24" s="18"/>
@@ -1342,65 +1551,46 @@
       <c r="G24" s="18"/>
       <c r="H24" s="18"/>
     </row>
-    <row r="25" spans="1:14" ht="21" x14ac:dyDescent="0.2">
-      <c r="B25" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="C25" s="44"/>
-      <c r="D25" s="44"/>
+    <row r="25" spans="1:14">
+      <c r="C25" s="34"/>
+      <c r="D25" s="34"/>
       <c r="E25" s="18"/>
       <c r="F25" s="18"/>
       <c r="G25" s="18"/>
       <c r="H25" s="18"/>
     </row>
-    <row r="26" spans="1:14" ht="21" x14ac:dyDescent="0.2">
-      <c r="B26" s="46" t="s">
-        <v>37</v>
-      </c>
-      <c r="C26" s="44"/>
-      <c r="D26" s="44"/>
+    <row r="26" spans="1:14">
+      <c r="C26" s="34"/>
+      <c r="D26" s="34"/>
       <c r="E26" s="18"/>
       <c r="F26" s="18"/>
       <c r="G26" s="18"/>
       <c r="H26" s="18"/>
     </row>
-    <row r="27" spans="1:14" ht="21" x14ac:dyDescent="0.2">
-      <c r="B27" s="47" t="s">
-        <v>38</v>
-      </c>
-      <c r="C27" s="44"/>
-      <c r="D27" s="44"/>
+    <row r="27" spans="1:14">
+      <c r="C27" s="34"/>
+      <c r="D27" s="34"/>
       <c r="E27" s="18"/>
       <c r="F27" s="18"/>
       <c r="G27" s="18"/>
       <c r="H27" s="18"/>
     </row>
-    <row r="28" spans="1:14" ht="21" x14ac:dyDescent="0.2">
-      <c r="B28" s="48" t="s">
-        <v>6</v>
-      </c>
-      <c r="C28" s="44"/>
-      <c r="D28" s="44"/>
+    <row r="28" spans="1:14">
+      <c r="C28" s="34"/>
+      <c r="D28" s="34"/>
       <c r="E28" s="18"/>
       <c r="F28" s="18"/>
       <c r="G28" s="18"/>
       <c r="H28" s="18"/>
     </row>
-    <row r="29" spans="1:14" ht="21" x14ac:dyDescent="0.2">
-      <c r="B29" s="49" t="s">
-        <v>5</v>
-      </c>
+    <row r="29" spans="1:14">
       <c r="C29" s="18"/>
       <c r="D29" s="18"/>
       <c r="E29" s="18"/>
     </row>
-    <row r="30" spans="1:14" ht="21" x14ac:dyDescent="0.2">
-      <c r="B30" s="50" t="s">
-        <v>39</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="A4:A13"/>
     <mergeCell ref="C22:E22"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="E14:E15"/>
@@ -1408,7 +1598,6 @@
     <mergeCell ref="G2:L2"/>
     <mergeCell ref="C20:E20"/>
     <mergeCell ref="C21:E21"/>
-    <mergeCell ref="A4:A13"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Forgot to update user stories left
Updated user stories left
</commit_message>
<xml_diff>
--- a/Sprint 2/Sprint_Backlog/Sprint 2 Backlog .xlsx
+++ b/Sprint 2/Sprint_Backlog/Sprint 2 Backlog .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stormfront/Desktop/GITHUB/Sites/DCDLEAFY.github.io/Sprint 2/Sprint_Backlog/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98666094-9DFF-3C47-AA2E-532CF562B1AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB55DA6D-ED03-F349-AFA8-A03689C676FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="220" yWindow="460" windowWidth="25380" windowHeight="14440" xr2:uid="{534C34EA-1E67-7A49-A34F-DDDABC004054}"/>
   </bookViews>
@@ -1018,6 +1018,9 @@
     <xf numFmtId="20" fontId="0" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1047,9 +1050,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1367,8 +1367,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B87E7FF6-10D9-A640-9FCB-92C9939F9B69}">
   <dimension ref="A2:N29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="110" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1392,21 +1392,21 @@
       <c r="B2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="46" t="s">
+      <c r="C2" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
       <c r="F2" s="25"/>
-      <c r="G2" s="51" t="s">
+      <c r="G2" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="49" t="s">
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="52"/>
+      <c r="M2" s="50" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1444,10 +1444,10 @@
       <c r="L3" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="M3" s="50"/>
+      <c r="M3" s="51"/>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="43" t="s">
         <v>18</v>
       </c>
       <c r="B4" s="27" t="s">
@@ -1476,7 +1476,7 @@
       <c r="M4" s="16"/>
     </row>
     <row r="5" spans="1:13">
-      <c r="A5" s="43"/>
+      <c r="A5" s="44"/>
       <c r="B5" s="28" t="s">
         <v>21</v>
       </c>
@@ -1505,7 +1505,7 @@
       <c r="M5" s="15"/>
     </row>
     <row r="6" spans="1:13">
-      <c r="A6" s="43"/>
+      <c r="A6" s="44"/>
       <c r="B6" s="29" t="s">
         <v>22</v>
       </c>
@@ -1530,7 +1530,7 @@
       <c r="M6" s="16"/>
     </row>
     <row r="7" spans="1:13">
-      <c r="A7" s="43"/>
+      <c r="A7" s="44"/>
       <c r="B7" s="28" t="s">
         <v>23</v>
       </c>
@@ -1557,7 +1557,7 @@
       <c r="M7" s="15"/>
     </row>
     <row r="8" spans="1:13">
-      <c r="A8" s="43"/>
+      <c r="A8" s="44"/>
       <c r="B8" s="29" t="s">
         <v>24</v>
       </c>
@@ -1580,7 +1580,7 @@
       <c r="M8" s="16"/>
     </row>
     <row r="9" spans="1:13">
-      <c r="A9" s="43"/>
+      <c r="A9" s="44"/>
       <c r="B9" s="28" t="s">
         <v>25</v>
       </c>
@@ -1607,7 +1607,7 @@
       <c r="M9" s="15"/>
     </row>
     <row r="10" spans="1:13">
-      <c r="A10" s="43"/>
+      <c r="A10" s="44"/>
       <c r="B10" s="29" t="s">
         <v>26</v>
       </c>
@@ -1632,7 +1632,7 @@
       <c r="M10" s="16"/>
     </row>
     <row r="11" spans="1:13">
-      <c r="A11" s="43"/>
+      <c r="A11" s="44"/>
       <c r="B11" s="28" t="s">
         <v>27</v>
       </c>
@@ -1659,7 +1659,7 @@
       <c r="M11" s="15"/>
     </row>
     <row r="12" spans="1:13">
-      <c r="A12" s="43"/>
+      <c r="A12" s="44"/>
       <c r="B12" s="29" t="s">
         <v>28</v>
       </c>
@@ -1686,7 +1686,7 @@
       <c r="M12" s="16"/>
     </row>
     <row r="13" spans="1:13">
-      <c r="A13" s="44"/>
+      <c r="A13" s="45"/>
       <c r="B13" s="30" t="s">
         <v>29</v>
       </c>
@@ -1712,7 +1712,7 @@
       <c r="A14" s="31"/>
       <c r="C14" s="21"/>
       <c r="D14" s="21"/>
-      <c r="E14" s="47" t="s">
+      <c r="E14" s="48" t="s">
         <v>17</v>
       </c>
       <c r="F14" s="23" t="s">
@@ -1736,7 +1736,7 @@
       <c r="A15" s="31"/>
       <c r="C15" s="20"/>
       <c r="D15" s="20"/>
-      <c r="E15" s="48"/>
+      <c r="E15" s="49"/>
       <c r="F15" s="24">
         <f>SUM(D4:D13)</f>
         <v>40</v>
@@ -1748,12 +1748,11 @@
         <v>21</v>
       </c>
       <c r="I15" s="22">
-        <f>H15-SUM(I4:I13)</f>
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="J15" s="24">
         <f>I15-SUM(J4:J13)</f>
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="K15" s="20"/>
       <c r="L15" s="12" t="s">
@@ -1805,28 +1804,28 @@
     </row>
     <row r="20" spans="1:14" ht="21">
       <c r="B20" s="13"/>
-      <c r="C20" s="45"/>
-      <c r="D20" s="45"/>
-      <c r="E20" s="45"/>
+      <c r="C20" s="46"/>
+      <c r="D20" s="46"/>
+      <c r="E20" s="46"/>
       <c r="L20" s="37" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="21">
       <c r="B21" s="13"/>
-      <c r="C21" s="45"/>
-      <c r="D21" s="45"/>
-      <c r="E21" s="45"/>
-      <c r="L21" s="52" t="s">
+      <c r="C21" s="46"/>
+      <c r="D21" s="46"/>
+      <c r="E21" s="46"/>
+      <c r="L21" s="42" t="s">
         <v>33</v>
       </c>
       <c r="N21" s="18"/>
     </row>
     <row r="22" spans="1:14">
       <c r="B22" s="13"/>
-      <c r="C22" s="45"/>
-      <c r="D22" s="45"/>
-      <c r="E22" s="45"/>
+      <c r="C22" s="46"/>
+      <c r="D22" s="46"/>
+      <c r="E22" s="46"/>
       <c r="N22" s="18"/>
     </row>
     <row r="23" spans="1:14">

</xml_diff>